<commit_message>
temporal: delete unused and old function for temporal disaggregation of application data_in: update database for application disaggregation per industrial branch
</commit_message>
<xml_diff>
--- a/data_in/dimensionless/application_disaggreagtion_keys.xlsx
+++ b/data_in/dimensionless/application_disaggreagtion_keys.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="690" windowWidth="19440" windowHeight="15000" tabRatio="808" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="690" windowWidth="19440" windowHeight="15000" tabRatio="808" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Namen WZ" sheetId="5" r:id="rId1"/>
@@ -623,7 +623,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -700,6 +700,7 @@
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -1814,7 +1815,7 @@
   </sheetPr>
   <dimension ref="A1:O111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
@@ -4729,8 +4730,8 @@
   </sheetPr>
   <dimension ref="A1:N146"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:J1048576"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4741,7 +4742,7 @@
     <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>95</v>
       </c>
@@ -4758,12 +4759,12 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>1</v>
       </c>
@@ -4779,8 +4780,9 @@
       <c r="E3" s="20">
         <v>5.6022408963585429E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="38"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>2</v>
       </c>
@@ -4796,8 +4798,9 @@
       <c r="E4" s="20">
         <v>5.6022408963585429E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="38"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>3</v>
       </c>
@@ -4813,8 +4816,9 @@
       <c r="E5" s="20">
         <v>6.6666666666666666E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="38"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>97</v>
       </c>
@@ -4822,8 +4826,9 @@
       <c r="C6" s="20"/>
       <c r="D6" s="20"/>
       <c r="E6" s="20"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="38"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>5</v>
       </c>
@@ -4839,8 +4844,9 @@
       <c r="E7" s="20">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="38"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>6</v>
       </c>
@@ -4856,8 +4862,9 @@
       <c r="E8" s="20">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="38"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>7</v>
       </c>
@@ -4873,8 +4880,9 @@
       <c r="E9" s="20">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="38"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>8</v>
       </c>
@@ -4890,8 +4898,9 @@
       <c r="E10" s="20">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="38"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>9</v>
       </c>
@@ -4907,8 +4916,9 @@
       <c r="E11" s="20">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="38"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>98</v>
       </c>
@@ -4916,8 +4926,9 @@
       <c r="C12" s="36"/>
       <c r="D12" s="36"/>
       <c r="E12" s="36"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="38"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>10</v>
       </c>
@@ -4933,8 +4944,9 @@
       <c r="E13" s="20">
         <v>9.9009900990099028E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="38"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>11</v>
       </c>
@@ -4950,8 +4962,9 @@
       <c r="E14" s="20">
         <v>9.9009900990099028E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="38"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>12</v>
       </c>
@@ -4967,8 +4980,9 @@
       <c r="E15" s="20">
         <v>9.9009900990099028E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="38"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>13</v>
       </c>
@@ -4984,6 +4998,7 @@
       <c r="E16" s="20">
         <v>2.7906976744186046E-2</v>
       </c>
+      <c r="F16" s="38"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
@@ -5001,6 +5016,7 @@
       <c r="E17" s="20">
         <v>2.7906976744186046E-2</v>
       </c>
+      <c r="F17" s="38"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
@@ -5018,6 +5034,7 @@
       <c r="E18" s="20">
         <v>2.7906976744186046E-2</v>
       </c>
+      <c r="F18" s="38"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
@@ -5035,6 +5052,7 @@
       <c r="E19" s="20">
         <v>2.7906976744186046E-2</v>
       </c>
+      <c r="F19" s="38"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
@@ -5052,6 +5070,7 @@
       <c r="E20" s="20">
         <v>2.5157232704402519E-3</v>
       </c>
+      <c r="F20" s="38"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
@@ -5069,7 +5088,7 @@
       <c r="E21" s="20">
         <v>2.7906976744186046E-2</v>
       </c>
-      <c r="F21" s="19"/>
+      <c r="F21" s="38"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
@@ -5087,6 +5106,7 @@
       <c r="E22" s="20">
         <v>0.01</v>
       </c>
+      <c r="F22" s="38"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
@@ -5104,6 +5124,7 @@
       <c r="E23" s="20">
         <v>1.1494252873563218E-3</v>
       </c>
+      <c r="F23" s="38"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
@@ -5121,7 +5142,7 @@
       <c r="E24" s="20">
         <v>9.433962264150943E-3</v>
       </c>
-      <c r="F24" s="19"/>
+      <c r="F24" s="38"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
@@ -5139,6 +5160,7 @@
       <c r="E25" s="20">
         <v>3.1674208144796379E-2</v>
       </c>
+      <c r="F25" s="38"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
@@ -5156,6 +5178,7 @@
       <c r="E26" s="20">
         <v>2.8818443804034589E-3</v>
       </c>
+      <c r="F26" s="38"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
@@ -5173,6 +5196,7 @@
       <c r="E27" s="20">
         <v>4.9721921929744579E-3</v>
       </c>
+      <c r="F27" s="38"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
@@ -5190,6 +5214,7 @@
       <c r="E28" s="20">
         <v>3.325942350332594E-2</v>
       </c>
+      <c r="F28" s="38"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
@@ -5207,6 +5232,7 @@
       <c r="E29" s="20">
         <v>2.7906976744186046E-2</v>
       </c>
+      <c r="F29" s="38"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
@@ -5224,6 +5250,7 @@
       <c r="E30" s="20">
         <v>2.7906976744186046E-2</v>
       </c>
+      <c r="F30" s="38"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
@@ -5241,6 +5268,7 @@
       <c r="E31" s="20">
         <v>8.2608695652173908E-2</v>
       </c>
+      <c r="F31" s="38"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
@@ -5258,6 +5286,7 @@
       <c r="E32" s="20">
         <v>4.1208791208791208E-2</v>
       </c>
+      <c r="F32" s="38"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
@@ -5275,6 +5304,7 @@
       <c r="E33" s="20">
         <v>4.1208791208791208E-2</v>
       </c>
+      <c r="F33" s="38"/>
       <c r="G33" s="23"/>
       <c r="H33" s="23"/>
       <c r="I33" s="23"/>
@@ -5300,6 +5330,7 @@
       <c r="E34" s="20">
         <v>2.7906976744186046E-2</v>
       </c>
+      <c r="F34" s="38"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="9">
@@ -5317,6 +5348,7 @@
       <c r="E35" s="20">
         <v>2.790697674418605E-2</v>
       </c>
+      <c r="F35" s="38"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
@@ -5334,6 +5366,7 @@
       <c r="E36" s="20">
         <v>2.7906976744186046E-2</v>
       </c>
+      <c r="F36" s="38"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
@@ -5343,6 +5376,7 @@
       <c r="C37" s="20"/>
       <c r="D37" s="20"/>
       <c r="E37" s="20"/>
+      <c r="F37" s="38"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
@@ -5352,6 +5386,7 @@
       <c r="C38" s="20"/>
       <c r="D38" s="20"/>
       <c r="E38" s="20"/>
+      <c r="F38" s="38"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
@@ -5361,6 +5396,7 @@
       <c r="C39" s="20"/>
       <c r="D39" s="20"/>
       <c r="E39" s="20"/>
+      <c r="F39" s="38"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
@@ -5378,6 +5414,7 @@
       <c r="E40" s="20">
         <v>0</v>
       </c>
+      <c r="F40" s="38"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
@@ -5395,6 +5432,7 @@
       <c r="E41" s="20">
         <v>0</v>
       </c>
+      <c r="F41" s="38"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
@@ -5412,6 +5450,7 @@
       <c r="E42" s="20">
         <v>3.5135135135135137E-2</v>
       </c>
+      <c r="F42" s="38"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
@@ -5429,6 +5468,7 @@
       <c r="E43" s="20">
         <v>3.5135135135135137E-2</v>
       </c>
+      <c r="F43" s="38"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
@@ -5438,6 +5478,7 @@
       <c r="C44" s="20"/>
       <c r="D44" s="20"/>
       <c r="E44" s="20"/>
+      <c r="F44" s="38"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="9">
@@ -5455,6 +5496,7 @@
       <c r="E45" s="20">
         <v>3.7313432835820892E-2</v>
       </c>
+      <c r="F45" s="38"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
@@ -5472,6 +5514,7 @@
       <c r="E46" s="20">
         <v>3.7313432835820892E-2</v>
       </c>
+      <c r="F46" s="38"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="9">
@@ -5489,6 +5532,7 @@
       <c r="E47" s="20">
         <v>3.7313432835820892E-2</v>
       </c>
+      <c r="F47" s="38"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
@@ -5498,8 +5542,9 @@
       <c r="C48" s="20"/>
       <c r="D48" s="20"/>
       <c r="E48" s="20"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48" s="38"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="9">
         <v>45</v>
       </c>
@@ -5515,8 +5560,9 @@
       <c r="E49" s="20">
         <v>3.2019704433497539E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49" s="38"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="9">
         <v>46</v>
       </c>
@@ -5532,8 +5578,9 @@
       <c r="E50" s="20">
         <v>3.2019704433497539E-2</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50" s="38"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="9">
         <v>47</v>
       </c>
@@ -5549,8 +5596,9 @@
       <c r="E51" s="20">
         <v>3.2019704433497539E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51" s="38"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="15" t="s">
         <v>102</v>
       </c>
@@ -5558,8 +5606,9 @@
       <c r="C52" s="20"/>
       <c r="D52" s="20"/>
       <c r="E52" s="20"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52" s="38"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="9">
         <v>49</v>
       </c>
@@ -5575,8 +5624,9 @@
       <c r="E53" s="20">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53" s="38"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="9">
         <v>50</v>
       </c>
@@ -5592,8 +5642,9 @@
       <c r="E54" s="20">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54" s="38"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="9">
         <v>51</v>
       </c>
@@ -5609,8 +5660,9 @@
       <c r="E55" s="20">
         <v>4.7619047619047616E-2</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55" s="38"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="9">
         <v>52</v>
       </c>
@@ -5626,8 +5678,9 @@
       <c r="E56" s="20">
         <v>2.2727272727272728E-2</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56" s="38"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="9">
         <v>53</v>
       </c>
@@ -5643,8 +5696,9 @@
       <c r="E57" s="20">
         <v>3.5135135135135137E-2</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57" s="38"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="15" t="s">
         <v>103</v>
       </c>
@@ -5652,8 +5706,9 @@
       <c r="C58" s="20"/>
       <c r="D58" s="20"/>
       <c r="E58" s="20"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F58" s="38"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="9">
         <v>55</v>
       </c>
@@ -5669,8 +5724,9 @@
       <c r="E59" s="20">
         <v>5.8568329718004339E-2</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F59" s="38"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="9">
         <v>56</v>
       </c>
@@ -5686,8 +5742,9 @@
       <c r="E60" s="20">
         <v>5.8568329718004339E-2</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F60" s="38"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="15" t="s">
         <v>104</v>
       </c>
@@ -5695,8 +5752,9 @@
       <c r="C61" s="20"/>
       <c r="D61" s="20"/>
       <c r="E61" s="20"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F61" s="38"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="9">
         <v>58</v>
       </c>
@@ -5712,8 +5770,9 @@
       <c r="E62" s="20">
         <v>3.5135135135135137E-2</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62" s="38"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="9">
         <v>59</v>
       </c>
@@ -5729,8 +5788,9 @@
       <c r="E63" s="20">
         <v>3.5135135135135137E-2</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F63" s="38"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="9">
         <v>60</v>
       </c>
@@ -5746,8 +5806,9 @@
       <c r="E64" s="20">
         <v>3.5135135135135137E-2</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64" s="38"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="9">
         <v>61</v>
       </c>
@@ -5763,8 +5824,9 @@
       <c r="E65" s="20">
         <v>3.5135135135135137E-2</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65" s="38"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="9">
         <v>62</v>
       </c>
@@ -5780,8 +5842,9 @@
       <c r="E66" s="20">
         <v>3.5135135135135137E-2</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66" s="38"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="9">
         <v>63</v>
       </c>
@@ -5797,8 +5860,9 @@
       <c r="E67" s="20">
         <v>3.5135135135135137E-2</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F67" s="38"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="15" t="s">
         <v>105</v>
       </c>
@@ -5806,8 +5870,9 @@
       <c r="C68" s="20"/>
       <c r="D68" s="20"/>
       <c r="E68" s="20"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68" s="38"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="9">
         <v>64</v>
       </c>
@@ -5823,8 +5888,9 @@
       <c r="E69" s="20">
         <v>3.5135135135135137E-2</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69" s="38"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="9">
         <v>65</v>
       </c>
@@ -5840,8 +5906,9 @@
       <c r="E70" s="20">
         <v>3.5135135135135137E-2</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70" s="38"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="9">
         <v>66</v>
       </c>
@@ -5857,8 +5924,9 @@
       <c r="E71" s="20">
         <v>3.5135135135135137E-2</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F71" s="38"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="15" t="s">
         <v>106</v>
       </c>
@@ -5866,8 +5934,9 @@
       <c r="C72" s="20"/>
       <c r="D72" s="20"/>
       <c r="E72" s="20"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F72" s="38"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="9">
         <v>68</v>
       </c>
@@ -5883,8 +5952,9 @@
       <c r="E73" s="20">
         <v>5.1056338028169015E-2</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F73" s="38"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="15" t="s">
         <v>117</v>
       </c>
@@ -5892,8 +5962,9 @@
       <c r="C74" s="20"/>
       <c r="D74" s="20"/>
       <c r="E74" s="20"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F74" s="38"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="9">
         <v>69</v>
       </c>
@@ -5909,8 +5980,9 @@
       <c r="E75" s="20">
         <v>3.5135135135135137E-2</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F75" s="38"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="9">
         <v>70</v>
       </c>
@@ -5926,8 +5998,9 @@
       <c r="E76" s="20">
         <v>3.5135135135135137E-2</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F76" s="38"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="9">
         <v>71</v>
       </c>
@@ -5943,8 +6016,9 @@
       <c r="E77" s="20">
         <v>3.5135135135135137E-2</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F77" s="38"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="9">
         <v>72</v>
       </c>
@@ -5960,8 +6034,9 @@
       <c r="E78" s="20">
         <v>3.5135135135135137E-2</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F78" s="38"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="9">
         <v>73</v>
       </c>
@@ -5977,8 +6052,9 @@
       <c r="E79" s="20">
         <v>3.5135135135135137E-2</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F79" s="38"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="9">
         <v>74</v>
       </c>
@@ -5994,8 +6070,9 @@
       <c r="E80" s="20">
         <v>3.5135135135135137E-2</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F80" s="38"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="9">
         <v>75</v>
       </c>
@@ -6011,8 +6088,9 @@
       <c r="E81" s="20">
         <v>5.1056338028169015E-2</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F81" s="38"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="15" t="s">
         <v>108</v>
       </c>
@@ -6020,8 +6098,9 @@
       <c r="C82" s="20"/>
       <c r="D82" s="20"/>
       <c r="E82" s="20"/>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F82" s="38"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="9">
         <v>77</v>
       </c>
@@ -6037,8 +6116,9 @@
       <c r="E83" s="20">
         <v>5.1056338028169015E-2</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F83" s="38"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="9">
         <v>78</v>
       </c>
@@ -6054,8 +6134,9 @@
       <c r="E84" s="20">
         <v>5.1056338028169015E-2</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F84" s="38"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="9">
         <v>79</v>
       </c>
@@ -6071,8 +6152,9 @@
       <c r="E85" s="20">
         <v>5.1056338028169015E-2</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F85" s="38"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="9">
         <v>80</v>
       </c>
@@ -6088,8 +6170,9 @@
       <c r="E86" s="20">
         <v>5.1056338028169015E-2</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F86" s="38"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="9">
         <v>81</v>
       </c>
@@ -6105,8 +6188,9 @@
       <c r="E87" s="20">
         <v>5.1056338028169015E-2</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F87" s="38"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="9">
         <v>82</v>
       </c>
@@ -6122,8 +6206,9 @@
       <c r="E88" s="20">
         <v>5.1056338028169015E-2</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F88" s="38"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="15" t="s">
         <v>109</v>
       </c>
@@ -6131,8 +6216,9 @@
       <c r="C89" s="20"/>
       <c r="D89" s="20"/>
       <c r="E89" s="20"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F89" s="38"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="9">
         <v>84</v>
       </c>
@@ -6148,8 +6234,9 @@
       <c r="E90" s="20">
         <v>3.5135135135135137E-2</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F90" s="38"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="15" t="s">
         <v>110</v>
       </c>
@@ -6157,8 +6244,9 @@
       <c r="C91" s="20"/>
       <c r="D91" s="20"/>
       <c r="E91" s="20"/>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F91" s="38"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="9">
         <v>85</v>
       </c>
@@ -6174,8 +6262,9 @@
       <c r="E92" s="20">
         <v>1.2048192771084336E-2</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F92" s="38"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="15" t="s">
         <v>111</v>
       </c>
@@ -6183,8 +6272,9 @@
       <c r="C93" s="20"/>
       <c r="D93" s="20"/>
       <c r="E93" s="20"/>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F93" s="38"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="9">
         <v>86</v>
       </c>
@@ -6200,8 +6290,9 @@
       <c r="E94" s="20">
         <v>0.15833333333333333</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F94" s="38"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="9">
         <v>87</v>
       </c>
@@ -6217,8 +6308,9 @@
       <c r="E95" s="20">
         <v>5.8568329718004339E-2</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F95" s="38"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="9">
         <v>88</v>
       </c>
@@ -6234,8 +6326,9 @@
       <c r="E96" s="20">
         <v>5.1056338028169015E-2</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F96" s="38"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="15" t="s">
         <v>112</v>
       </c>
@@ -6243,8 +6336,9 @@
       <c r="C97" s="20"/>
       <c r="D97" s="20"/>
       <c r="E97" s="20"/>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F97" s="38"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="9">
         <v>90</v>
       </c>
@@ -6260,8 +6354,9 @@
       <c r="E98" s="20">
         <v>5.1056338028169015E-2</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F98" s="38"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="9">
         <v>91</v>
       </c>
@@ -6277,8 +6372,9 @@
       <c r="E99" s="20">
         <v>5.1056338028169015E-2</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F99" s="38"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="9">
         <v>92</v>
       </c>
@@ -6294,8 +6390,9 @@
       <c r="E100" s="20">
         <v>5.1056338028169015E-2</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F100" s="38"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="9">
         <v>93</v>
       </c>
@@ -6311,8 +6408,9 @@
       <c r="E101" s="20">
         <v>5.1056338028169015E-2</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F101" s="38"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="15" t="s">
         <v>113</v>
       </c>
@@ -6320,8 +6418,9 @@
       <c r="C102" s="20"/>
       <c r="D102" s="20"/>
       <c r="E102" s="20"/>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F102" s="38"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="9">
         <v>94</v>
       </c>
@@ -6337,8 +6436,9 @@
       <c r="E103" s="20">
         <v>5.1056338028169015E-2</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F103" s="38"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="9">
         <v>95</v>
       </c>
@@ -6354,8 +6454,9 @@
       <c r="E104" s="20">
         <v>5.1056338028169015E-2</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F104" s="38"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="9">
         <v>96</v>
       </c>
@@ -6371,8 +6472,9 @@
       <c r="E105" s="20">
         <v>5.1056338028169015E-2</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F105" s="38"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="15" t="s">
         <v>118</v>
       </c>
@@ -6380,8 +6482,9 @@
       <c r="C106" s="20"/>
       <c r="D106" s="20"/>
       <c r="E106" s="20"/>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F106" s="38"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="9">
         <v>97</v>
       </c>
@@ -6397,8 +6500,9 @@
       <c r="E107" s="20">
         <v>5.1056338028169015E-2</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F107" s="38"/>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="9">
         <v>98</v>
       </c>
@@ -6414,8 +6518,9 @@
       <c r="E108" s="20">
         <v>5.1056338028169015E-2</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F108" s="38"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="15" t="s">
         <v>114</v>
       </c>
@@ -6423,8 +6528,9 @@
       <c r="C109" s="20"/>
       <c r="D109" s="20"/>
       <c r="E109" s="20"/>
-    </row>
-    <row r="110" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F109" s="38"/>
+    </row>
+    <row r="110" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="10">
         <v>99</v>
       </c>
@@ -6440,15 +6546,16 @@
       <c r="E110" s="20">
         <v>5.1056338028169015E-2</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F110" s="38"/>
+    </row>
+    <row r="111" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="11"/>
       <c r="B111" s="37"/>
       <c r="C111" s="36"/>
       <c r="D111" s="36"/>
       <c r="E111" s="36"/>
     </row>
-    <row r="112" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="18"/>
       <c r="B112" s="20"/>
       <c r="C112" s="20"/>
@@ -6671,8 +6778,8 @@
   </sheetPr>
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:XFD196"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>